<commit_message>
Expense Amount - CustAoumnt Index Error Solved
</commit_message>
<xml_diff>
--- a/Voltas_non_standard/Mysql/Area_mapping.xlsx
+++ b/Voltas_non_standard/Mysql/Area_mapping.xlsx
@@ -2833,12 +2833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" filterMode="1"/>
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K188"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2889,7 +2887,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>524305</v>
       </c>
@@ -2927,7 +2925,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>524240</v>
+        <v>524002</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -2939,29 +2937,28 @@
         <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I3" s="2">
-        <v>95</v>
+        <v>25.3</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J66" si="0">IF(I3&gt;75,290,IF(I3&gt;50,250,IF(I3&gt;25,150,0)))</f>
-        <v>290</v>
+        <v>100</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>524152</v>
       </c>
@@ -2990,14 +2987,14 @@
         <v>95</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I4&gt;75,290,IF(I4&gt;50,250,IF(I4&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>524001</v>
       </c>
@@ -3026,14 +3023,14 @@
         <v>15</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I5&gt;75,290,IF(I5&gt;50,250,IF(I5&gt;25,150,0)))</f>
         <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>524201</v>
       </c>
@@ -3062,14 +3059,14 @@
         <v>90</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I6&gt;75,290,IF(I6&gt;50,250,IF(I6&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>524202</v>
       </c>
@@ -3098,14 +3095,14 @@
         <v>90</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I7&gt;75,290,IF(I7&gt;50,250,IF(I7&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>524316</v>
       </c>
@@ -3134,14 +3131,14 @@
         <v>30</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I8&gt;75,290,IF(I8&gt;50,250,IF(I8&gt;25,150,0)))</f>
         <v>150</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>524344</v>
       </c>
@@ -3170,7 +3167,7 @@
         <v>90</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I9&gt;75,290,IF(I9&gt;50,250,IF(I9&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -3179,7 +3176,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>524313</v>
+        <v>524302</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
@@ -3191,10 +3188,10 @@
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>13</v>
@@ -3203,11 +3200,11 @@
         <v>18</v>
       </c>
       <c r="I10" s="2">
-        <v>52.5</v>
+        <v>107.5</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" si="0"/>
-        <v>250</v>
+        <f>IF(I10&gt;75,290,IF(I10&gt;50,250,IF(I10&gt;25,150,0)))</f>
+        <v>290</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>121</v>
@@ -3215,7 +3212,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>524230</v>
+        <v>524004</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>8</v>
@@ -3227,23 +3224,22 @@
         <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I11" s="2">
-        <v>90</v>
+        <v>25.3</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="0"/>
-        <v>290</v>
+        <v>100</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>121</v>
@@ -3251,7 +3247,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>524002</v>
+        <v>524304</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>8</v>
@@ -3266,25 +3262,26 @@
         <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I12" s="2">
-        <v>25.3</v>
+        <v>80</v>
       </c>
       <c r="J12" s="2">
-        <v>100</v>
+        <f>IF(I12&gt;75,290,IF(I12&gt;50,250,IF(I12&gt;25,150,0)))</f>
+        <v>290</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>524003</v>
       </c>
@@ -3313,7 +3310,7 @@
         <v>15</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I13&gt;75,290,IF(I13&gt;50,250,IF(I13&gt;25,150,0)))</f>
         <v>0</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -3322,7 +3319,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>524004</v>
+        <v>524322</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>8</v>
@@ -3337,19 +3334,20 @@
         <v>9</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I14" s="2">
-        <v>25.3</v>
+        <v>80</v>
       </c>
       <c r="J14" s="2">
-        <v>100</v>
+        <f>IF(I14&gt;75,290,IF(I14&gt;50,250,IF(I14&gt;25,150,0)))</f>
+        <v>290</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>121</v>
@@ -3357,7 +3355,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>524005</v>
+        <v>524310</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
@@ -3369,29 +3367,29 @@
         <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I15" s="2">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(I15&gt;75,290,IF(I15&gt;50,250,IF(I15&gt;25,150,0)))</f>
+        <v>290</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>524006</v>
       </c>
@@ -3420,14 +3418,14 @@
         <v>27.5</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I16&gt;75,290,IF(I16&gt;50,250,IF(I16&gt;25,150,0)))</f>
         <v>150</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>524137</v>
       </c>
@@ -3456,14 +3454,14 @@
         <v>30</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I17&gt;75,290,IF(I17&gt;50,250,IF(I17&gt;25,150,0)))</f>
         <v>150</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>524142</v>
       </c>
@@ -3492,14 +3490,14 @@
         <v>76.5</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I18&gt;75,290,IF(I18&gt;50,250,IF(I18&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>524203</v>
       </c>
@@ -3528,14 +3526,14 @@
         <v>85</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I19&gt;75,290,IF(I19&gt;50,250,IF(I19&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>524221</v>
       </c>
@@ -3564,7 +3562,7 @@
         <v>115</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I20&gt;75,290,IF(I20&gt;50,250,IF(I20&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K20" s="2" t="s">
@@ -3573,7 +3571,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>524222</v>
+        <v>524230</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>8</v>
@@ -3585,10 +3583,10 @@
         <v>9</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>13</v>
@@ -3597,17 +3595,17 @@
         <v>18</v>
       </c>
       <c r="I21" s="2">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I21&gt;75,290,IF(I21&gt;50,250,IF(I21&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>524223</v>
       </c>
@@ -3636,7 +3634,7 @@
         <v>80</v>
       </c>
       <c r="J22" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I22&gt;75,290,IF(I22&gt;50,250,IF(I22&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K22" s="2" t="s">
@@ -3645,7 +3643,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>524224</v>
+        <v>524240</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>8</v>
@@ -3657,10 +3655,10 @@
         <v>9</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>13</v>
@@ -3672,7 +3670,7 @@
         <v>95</v>
       </c>
       <c r="J23" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I23&gt;75,290,IF(I23&gt;50,250,IF(I23&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K23" s="2" t="s">
@@ -3681,7 +3679,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>524226</v>
+        <v>524346</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>8</v>
@@ -3696,7 +3694,7 @@
         <v>9</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>13</v>
@@ -3705,17 +3703,17 @@
         <v>18</v>
       </c>
       <c r="I24" s="2">
-        <v>140</v>
+        <v>52.5</v>
       </c>
       <c r="J24" s="2">
-        <f t="shared" si="0"/>
-        <v>290</v>
+        <f>IF(I24&gt;75,290,IF(I24&gt;50,250,IF(I24&gt;25,150,0)))</f>
+        <v>250</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>524227</v>
       </c>
@@ -3744,14 +3742,14 @@
         <v>145</v>
       </c>
       <c r="J25" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I25&gt;75,290,IF(I25&gt;50,250,IF(I25&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>524228</v>
       </c>
@@ -3780,7 +3778,7 @@
         <v>100</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I26&gt;75,290,IF(I26&gt;50,250,IF(I26&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K26" s="2" t="s">
@@ -3789,7 +3787,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>524234</v>
+        <v>524222</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>8</v>
@@ -3804,7 +3802,7 @@
         <v>9</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>13</v>
@@ -3813,19 +3811,19 @@
         <v>18</v>
       </c>
       <c r="I27" s="2">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="J27" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I27&gt;75,290,IF(I27&gt;50,250,IF(I27&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>524236</v>
+        <v>524317</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>8</v>
@@ -3840,28 +3838,28 @@
         <v>9</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I28" s="2">
-        <v>145</v>
+        <v>40</v>
       </c>
       <c r="J28" s="2">
-        <f t="shared" si="0"/>
-        <v>290</v>
+        <f>IF(I28&gt;75,290,IF(I28&gt;50,250,IF(I28&gt;25,150,0)))</f>
+        <v>150</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>524302</v>
+        <v>524236</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>8</v>
@@ -3876,7 +3874,7 @@
         <v>9</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>13</v>
@@ -3885,10 +3883,10 @@
         <v>18</v>
       </c>
       <c r="I29" s="2">
-        <v>107.5</v>
+        <v>145</v>
       </c>
       <c r="J29" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I29&gt;75,290,IF(I29&gt;50,250,IF(I29&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K29" s="2" t="s">
@@ -3897,7 +3895,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>524303</v>
+        <v>524407</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>8</v>
@@ -3912,7 +3910,7 @@
         <v>9</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>13</v>
@@ -3921,19 +3919,19 @@
         <v>18</v>
       </c>
       <c r="I30" s="2">
-        <v>95</v>
+        <v>76.5</v>
       </c>
       <c r="J30" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I30&gt;75,290,IF(I30&gt;50,250,IF(I30&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>524304</v>
+        <v>524234</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>8</v>
@@ -3948,7 +3946,7 @@
         <v>9</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>13</v>
@@ -3957,17 +3955,17 @@
         <v>18</v>
       </c>
       <c r="I31" s="2">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I31&gt;75,290,IF(I31&gt;50,250,IF(I31&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>524306</v>
       </c>
@@ -3996,7 +3994,7 @@
         <v>27.5</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I32&gt;75,290,IF(I32&gt;50,250,IF(I32&gt;25,150,0)))</f>
         <v>150</v>
       </c>
       <c r="K32" s="2" t="s">
@@ -4005,7 +4003,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>524307</v>
+        <v>524409</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>8</v>
@@ -4020,7 +4018,7 @@
         <v>9</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>13</v>
@@ -4029,10 +4027,10 @@
         <v>18</v>
       </c>
       <c r="I33" s="2">
-        <v>100</v>
+        <v>77.5</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I33&gt;75,290,IF(I33&gt;50,250,IF(I33&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K33" s="2" t="s">
@@ -4041,7 +4039,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>524309</v>
+        <v>524224</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>8</v>
@@ -4056,7 +4054,7 @@
         <v>9</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>13</v>
@@ -4065,17 +4063,17 @@
         <v>18</v>
       </c>
       <c r="I34" s="2">
-        <v>51.5</v>
+        <v>95</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" si="0"/>
-        <v>250</v>
+        <f>IF(I34&gt;75,290,IF(I34&gt;50,250,IF(I34&gt;25,150,0)))</f>
+        <v>290</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>524311</v>
       </c>
@@ -4104,7 +4102,7 @@
         <v>26.5</v>
       </c>
       <c r="J35" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I35&gt;75,290,IF(I35&gt;50,250,IF(I35&gt;25,150,0)))</f>
         <v>150</v>
       </c>
       <c r="K35" s="2" t="s">
@@ -4113,7 +4111,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>524312</v>
+        <v>524343</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>8</v>
@@ -4128,7 +4126,7 @@
         <v>9</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>13</v>
@@ -4137,17 +4135,17 @@
         <v>18</v>
       </c>
       <c r="I36" s="2">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="J36" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I36&gt;75,290,IF(I36&gt;50,250,IF(I36&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>524315</v>
       </c>
@@ -4176,7 +4174,7 @@
         <v>55</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I37&gt;75,290,IF(I37&gt;50,250,IF(I37&gt;25,150,0)))</f>
         <v>250</v>
       </c>
       <c r="K37" s="2" t="s">
@@ -4185,7 +4183,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>524317</v>
+        <v>524307</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>8</v>
@@ -4200,28 +4198,28 @@
         <v>9</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I38" s="2">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" si="0"/>
-        <v>150</v>
+        <f>IF(I38&gt;75,290,IF(I38&gt;50,250,IF(I38&gt;25,150,0)))</f>
+        <v>290</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>524322</v>
+        <v>524333</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>8</v>
@@ -4236,7 +4234,7 @@
         <v>9</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>13</v>
@@ -4245,17 +4243,17 @@
         <v>18</v>
       </c>
       <c r="I39" s="2">
-        <v>80</v>
+        <v>53.5</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" si="0"/>
-        <v>290</v>
+        <f>IF(I39&gt;75,290,IF(I39&gt;50,250,IF(I39&gt;25,150,0)))</f>
+        <v>250</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>524323</v>
       </c>
@@ -4284,14 +4282,14 @@
         <v>35</v>
       </c>
       <c r="J40" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I40&gt;75,290,IF(I40&gt;50,250,IF(I40&gt;25,150,0)))</f>
         <v>150</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>524324</v>
       </c>
@@ -4320,7 +4318,7 @@
         <v>125</v>
       </c>
       <c r="J41" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I41&gt;75,290,IF(I41&gt;50,250,IF(I41&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K41" s="2" t="s">
@@ -4329,7 +4327,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>524333</v>
+        <v>524301</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>8</v>
@@ -4341,31 +4339,31 @@
         <v>9</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="F42" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" s="2">
         <v>85</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I42" s="2">
-        <v>53.5</v>
-      </c>
       <c r="J42" s="2">
-        <f t="shared" si="0"/>
-        <v>250</v>
+        <f>IF(I42&gt;75,290,IF(I42&gt;50,250,IF(I42&gt;25,150,0)))</f>
+        <v>290</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>524343</v>
+        <v>524312</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>8</v>
@@ -4380,7 +4378,7 @@
         <v>9</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>13</v>
@@ -4389,10 +4387,10 @@
         <v>18</v>
       </c>
       <c r="I43" s="2">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="J43" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I43&gt;75,290,IF(I43&gt;50,250,IF(I43&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K43" s="2" t="s">
@@ -4401,7 +4399,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>524345</v>
+        <v>524005</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>8</v>
@@ -4416,7 +4414,7 @@
         <v>9</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>13</v>
@@ -4425,19 +4423,19 @@
         <v>12</v>
       </c>
       <c r="I44" s="2">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="J44" s="2">
-        <f t="shared" si="0"/>
-        <v>250</v>
+        <f>IF(I44&gt;75,290,IF(I44&gt;50,250,IF(I44&gt;25,150,0)))</f>
+        <v>0</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>524346</v>
+        <v>524313</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>8</v>
@@ -4449,10 +4447,10 @@
         <v>9</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>13</v>
@@ -4464,14 +4462,14 @@
         <v>52.5</v>
       </c>
       <c r="J45" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I45&gt;75,290,IF(I45&gt;50,250,IF(I45&gt;25,150,0)))</f>
         <v>250</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>524366</v>
       </c>
@@ -4500,7 +4498,7 @@
         <v>35</v>
       </c>
       <c r="J46" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I46&gt;75,290,IF(I46&gt;50,250,IF(I46&gt;25,150,0)))</f>
         <v>150</v>
       </c>
       <c r="K46" s="2" t="s">
@@ -4509,7 +4507,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>524407</v>
+        <v>524408</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>8</v>
@@ -4524,7 +4522,7 @@
         <v>9</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>13</v>
@@ -4533,10 +4531,10 @@
         <v>18</v>
       </c>
       <c r="I47" s="2">
-        <v>76.5</v>
+        <v>77.5</v>
       </c>
       <c r="J47" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I47&gt;75,290,IF(I47&gt;50,250,IF(I47&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K47" s="2" t="s">
@@ -4545,7 +4543,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>524408</v>
+        <v>524303</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>8</v>
@@ -4560,28 +4558,28 @@
         <v>9</v>
       </c>
       <c r="F48" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48" s="2">
         <v>95</v>
       </c>
-      <c r="G48" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I48" s="2">
-        <v>77.5</v>
-      </c>
       <c r="J48" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I48&gt;75,290,IF(I48&gt;50,250,IF(I48&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>524409</v>
+        <v>524321</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>8</v>
@@ -4593,10 +4591,10 @@
         <v>9</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>13</v>
@@ -4605,11 +4603,11 @@
         <v>18</v>
       </c>
       <c r="I49" s="2">
-        <v>77.5</v>
+        <v>40</v>
       </c>
       <c r="J49" s="2">
-        <f t="shared" si="0"/>
-        <v>290</v>
+        <f>IF(I49&gt;75,290,IF(I49&gt;50,250,IF(I49&gt;25,150,0)))</f>
+        <v>150</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>121</v>
@@ -4617,7 +4615,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>524308</v>
+        <v>524345</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>8</v>
@@ -4629,22 +4627,22 @@
         <v>9</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>102</v>
+        <v>9</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I50" s="2">
-        <v>53.5</v>
+        <v>55</v>
       </c>
       <c r="J50" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I50&gt;75,290,IF(I50&gt;50,250,IF(I50&gt;25,150,0)))</f>
         <v>250</v>
       </c>
       <c r="K50" s="2" t="s">
@@ -4653,7 +4651,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>524310</v>
+        <v>524225</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>8</v>
@@ -4665,10 +4663,10 @@
         <v>9</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>13</v>
@@ -4677,19 +4675,19 @@
         <v>18</v>
       </c>
       <c r="I51" s="2">
-        <v>140</v>
+        <v>77.5</v>
       </c>
       <c r="J51" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I51&gt;75,290,IF(I51&gt;50,250,IF(I51&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>524225</v>
+        <v>524226</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>8</v>
@@ -4701,10 +4699,10 @@
         <v>9</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>13</v>
@@ -4713,10 +4711,10 @@
         <v>18</v>
       </c>
       <c r="I52" s="2">
-        <v>77.5</v>
+        <v>140</v>
       </c>
       <c r="J52" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I52&gt;75,290,IF(I52&gt;50,250,IF(I52&gt;25,150,0)))</f>
         <v>290</v>
       </c>
       <c r="K52" s="2" t="s">
@@ -4725,7 +4723,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>524301</v>
+        <v>524308</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>8</v>
@@ -4737,10 +4735,10 @@
         <v>9</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>13</v>
@@ -4749,11 +4747,11 @@
         <v>18</v>
       </c>
       <c r="I53" s="2">
-        <v>85</v>
+        <v>53.5</v>
       </c>
       <c r="J53" s="2">
-        <f t="shared" si="0"/>
-        <v>290</v>
+        <f>IF(I53&gt;75,290,IF(I53&gt;50,250,IF(I53&gt;25,150,0)))</f>
+        <v>250</v>
       </c>
       <c r="K53" s="2" t="s">
         <v>118</v>
@@ -4761,7 +4759,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>524321</v>
+        <v>524309</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>8</v>
@@ -4773,10 +4771,10 @@
         <v>9</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>109</v>
+        <v>9</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>13</v>
@@ -4785,17 +4783,17 @@
         <v>18</v>
       </c>
       <c r="I54" s="2">
-        <v>40</v>
+        <v>51.5</v>
       </c>
       <c r="J54" s="2">
-        <f t="shared" si="0"/>
-        <v>150</v>
+        <f>IF(I54&gt;75,290,IF(I54&gt;50,250,IF(I54&gt;25,150,0)))</f>
+        <v>250</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>524218</v>
       </c>
@@ -4824,14 +4822,14 @@
         <v>55</v>
       </c>
       <c r="J55" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J3:J66" si="0">IF(I55&gt;75,290,IF(I55&gt;50,250,IF(I55&gt;25,150,0)))</f>
         <v>250</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>524341</v>
       </c>
@@ -4867,7 +4865,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>524412</v>
       </c>
@@ -4903,7 +4901,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>524403</v>
       </c>
@@ -4939,7 +4937,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>524134</v>
       </c>
@@ -4975,7 +4973,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>524410</v>
       </c>
@@ -5011,7 +5009,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>524126</v>
       </c>
@@ -5047,7 +5045,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>524101</v>
       </c>
@@ -5083,7 +5081,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>524102</v>
       </c>
@@ -5119,7 +5117,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>524119</v>
       </c>
@@ -5155,7 +5153,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>524120</v>
       </c>
@@ -5191,7 +5189,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>524121</v>
       </c>
@@ -5227,7 +5225,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>524123</v>
       </c>
@@ -5263,7 +5261,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>524124</v>
       </c>
@@ -5299,7 +5297,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>524127</v>
       </c>
@@ -5335,7 +5333,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>524129</v>
       </c>
@@ -5371,7 +5369,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>524131</v>
       </c>
@@ -5407,7 +5405,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>524132</v>
       </c>
@@ -5443,7 +5441,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>524401</v>
       </c>
@@ -5479,7 +5477,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>524402</v>
       </c>
@@ -5515,7 +5513,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>524404</v>
       </c>
@@ -5551,7 +5549,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>524405</v>
       </c>
@@ -5587,7 +5585,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>524411</v>
       </c>
@@ -5623,7 +5621,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>524414</v>
       </c>
@@ -5659,7 +5657,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>524421</v>
       </c>
@@ -5695,7 +5693,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>524441</v>
       </c>
@@ -5731,7 +5729,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>524624</v>
       </c>
@@ -5767,7 +5765,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>524415</v>
       </c>
@@ -5803,7 +5801,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>524320</v>
       </c>
@@ -5839,7 +5837,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>517502</v>
       </c>
@@ -5873,7 +5871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>517506</v>
       </c>
@@ -5906,7 +5904,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>517507</v>
       </c>
@@ -5940,7 +5938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>517590</v>
       </c>
@@ -5974,7 +5972,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>517551</v>
       </c>
@@ -6008,7 +6006,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>517277</v>
       </c>
@@ -6042,7 +6040,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>517001</v>
       </c>
@@ -6076,7 +6074,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>517423</v>
       </c>
@@ -6110,7 +6108,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>517613</v>
       </c>
@@ -6143,7 +6141,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>515412</v>
       </c>
@@ -6176,7 +6174,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>517002</v>
       </c>
@@ -6210,7 +6208,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>517003</v>
       </c>
@@ -6244,7 +6242,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>517004</v>
       </c>
@@ -6278,7 +6276,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>517101</v>
       </c>
@@ -6312,7 +6310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>517102</v>
       </c>
@@ -6346,7 +6344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>517112</v>
       </c>
@@ -6379,7 +6377,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>517113</v>
       </c>
@@ -6413,7 +6411,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>517123</v>
       </c>
@@ -6447,7 +6445,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>517124</v>
       </c>
@@ -6481,7 +6479,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>517125</v>
       </c>
@@ -6515,7 +6513,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>517126</v>
       </c>
@@ -6549,7 +6547,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>517127</v>
       </c>
@@ -6583,7 +6581,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>517128</v>
       </c>
@@ -6617,7 +6615,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>517129</v>
       </c>
@@ -6651,7 +6649,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>517130</v>
       </c>
@@ -6685,7 +6683,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>517131</v>
       </c>
@@ -6719,7 +6717,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>517132</v>
       </c>
@@ -6753,7 +6751,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>517150</v>
       </c>
@@ -6786,7 +6784,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>517152</v>
       </c>
@@ -6820,7 +6818,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>517167</v>
       </c>
@@ -6854,7 +6852,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>517172</v>
       </c>
@@ -6888,7 +6886,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>517192</v>
       </c>
@@ -6922,7 +6920,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>517193</v>
       </c>
@@ -6956,7 +6954,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>517194</v>
       </c>
@@ -6990,7 +6988,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>517198</v>
       </c>
@@ -7023,7 +7021,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>517213</v>
       </c>
@@ -7057,7 +7055,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>517214</v>
       </c>
@@ -7091,7 +7089,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>517234</v>
       </c>
@@ -7125,7 +7123,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>517235</v>
       </c>
@@ -7159,7 +7157,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>517236</v>
       </c>
@@ -7193,7 +7191,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>517237</v>
       </c>
@@ -7227,7 +7225,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>517247</v>
       </c>
@@ -7261,7 +7259,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>517257</v>
       </c>
@@ -7295,7 +7293,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>517280</v>
       </c>
@@ -7329,7 +7327,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>517291</v>
       </c>
@@ -7363,7 +7361,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>517297</v>
       </c>
@@ -7397,7 +7395,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>517299</v>
       </c>
@@ -7431,7 +7429,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>517302</v>
       </c>
@@ -7464,7 +7462,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>517305</v>
       </c>
@@ -7498,7 +7496,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>517319</v>
       </c>
@@ -7532,7 +7530,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>517325</v>
       </c>
@@ -7566,7 +7564,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>517326</v>
       </c>
@@ -7600,7 +7598,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>517327</v>
       </c>
@@ -7634,7 +7632,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>517350</v>
       </c>
@@ -7668,7 +7666,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>517351</v>
       </c>
@@ -7702,7 +7700,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>517352</v>
       </c>
@@ -7736,7 +7734,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>517370</v>
       </c>
@@ -7770,7 +7768,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>517390</v>
       </c>
@@ -7804,7 +7802,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>517391</v>
       </c>
@@ -7838,7 +7836,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>517403</v>
       </c>
@@ -7872,7 +7870,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>517408</v>
       </c>
@@ -7906,7 +7904,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>517414</v>
       </c>
@@ -7940,7 +7938,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>517415</v>
       </c>
@@ -7974,7 +7972,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>517416</v>
       </c>
@@ -8008,7 +8006,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>517417</v>
       </c>
@@ -8042,7 +8040,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>517418</v>
       </c>
@@ -8076,7 +8074,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>517419</v>
       </c>
@@ -8110,7 +8108,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>517421</v>
       </c>
@@ -8144,7 +8142,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>517422</v>
       </c>
@@ -8178,7 +8176,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>517424</v>
       </c>
@@ -8212,7 +8210,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="154" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>517425</v>
       </c>
@@ -8246,7 +8244,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>517429</v>
       </c>
@@ -8280,7 +8278,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>517432</v>
       </c>
@@ -8314,7 +8312,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>517503</v>
       </c>
@@ -8348,7 +8346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>517505</v>
       </c>
@@ -8382,7 +8380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>517517</v>
       </c>
@@ -8415,7 +8413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>517526</v>
       </c>
@@ -8449,7 +8447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>517536</v>
       </c>
@@ -8483,7 +8481,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>517541</v>
       </c>
@@ -8517,7 +8515,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>517561</v>
       </c>
@@ -8551,7 +8549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>517569</v>
       </c>
@@ -8585,7 +8583,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>517571</v>
       </c>
@@ -8619,7 +8617,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>517581</v>
       </c>
@@ -8653,7 +8651,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>517583</v>
       </c>
@@ -8687,7 +8685,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>517584</v>
       </c>
@@ -8721,7 +8719,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>517586</v>
       </c>
@@ -8755,7 +8753,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>517587</v>
       </c>
@@ -8789,7 +8787,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>517588</v>
       </c>
@@ -8823,7 +8821,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>517589</v>
       </c>
@@ -8857,7 +8855,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>517591</v>
       </c>
@@ -8891,7 +8889,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>517592</v>
       </c>
@@ -8925,7 +8923,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>517599</v>
       </c>
@@ -8959,7 +8957,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>517619</v>
       </c>
@@ -8993,7 +8991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>517620</v>
       </c>
@@ -9027,7 +9025,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>517640</v>
       </c>
@@ -9061,7 +9059,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>517641</v>
       </c>
@@ -9095,7 +9093,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="180" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>517642</v>
       </c>
@@ -9129,7 +9127,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>517643</v>
       </c>
@@ -9163,7 +9161,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="182" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>517644</v>
       </c>
@@ -9197,7 +9195,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="183" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>517582</v>
       </c>
@@ -9231,7 +9229,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="184" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>517401</v>
       </c>
@@ -9265,7 +9263,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="185" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>517520</v>
       </c>
@@ -9299,7 +9297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>517664</v>
       </c>
@@ -9332,7 +9330,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="187" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>517504</v>
       </c>
@@ -9365,7 +9363,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="188" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>517501</v>
       </c>
@@ -9400,11 +9398,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K188">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="AL MADINA ENTERPRISES"/>
-      </filters>
-    </filterColumn>
+    <sortState ref="A3:K54">
+      <sortCondition ref="F1:F188"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>